<commit_message>
GROW-28 fix : 배당금 header에 0 빠지는 오류 처리
</commit_message>
<xml_diff>
--- a/backend/etc/file/hongkong_stock_list.xlsx
+++ b/backend/etc/file/hongkong_stock_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
   <si>
     <t>Symbol</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Code</t>
   </si>
   <si>
+    <t>0001</t>
+  </si>
+  <si>
     <t>CK Hutchison Holdings</t>
   </si>
   <si>
@@ -34,73 +37,145 @@
     <t>HSI</t>
   </si>
   <si>
+    <t>0002</t>
+  </si>
+  <si>
     <t>CLP Holdings</t>
   </si>
   <si>
+    <t>0003</t>
+  </si>
+  <si>
     <t>Hong Kong &amp; China Gas</t>
   </si>
   <si>
+    <t>0005</t>
+  </si>
+  <si>
     <t>HSBC Holdings</t>
   </si>
   <si>
+    <t>0011</t>
+  </si>
+  <si>
     <t>Hang Seng Bank</t>
   </si>
   <si>
+    <t>0012</t>
+  </si>
+  <si>
     <t>Henderson Land Development</t>
   </si>
   <si>
+    <t>0016</t>
+  </si>
+  <si>
     <t>Sun Hung Kai Properties</t>
   </si>
   <si>
+    <t>0017</t>
+  </si>
+  <si>
     <t>New World Development</t>
   </si>
   <si>
+    <t>0019</t>
+  </si>
+  <si>
     <t>Swire Pacific</t>
   </si>
   <si>
+    <t>0023</t>
+  </si>
+  <si>
     <t>Bank of East Asia</t>
   </si>
   <si>
+    <t>0027</t>
+  </si>
+  <si>
     <t>Galaxy Entertainment Group</t>
   </si>
   <si>
+    <t>0066</t>
+  </si>
+  <si>
     <t>MTR Corporation</t>
   </si>
   <si>
+    <t>0101</t>
+  </si>
+  <si>
     <t>Hang Lung Properties</t>
   </si>
   <si>
+    <t>0388</t>
+  </si>
+  <si>
     <t>Hong Kong Exchanges and Clearing</t>
   </si>
   <si>
+    <t>0688</t>
+  </si>
+  <si>
     <t>China Overseas Land &amp; Investment</t>
   </si>
   <si>
+    <t>0700</t>
+  </si>
+  <si>
     <t>Tencent Holdings</t>
   </si>
   <si>
+    <t>0762</t>
+  </si>
+  <si>
     <t>China Unicom</t>
   </si>
   <si>
+    <t>0823</t>
+  </si>
+  <si>
     <t>Link REIT</t>
   </si>
   <si>
+    <t>0857</t>
+  </si>
+  <si>
     <t>PetroChina</t>
   </si>
   <si>
+    <t>0868</t>
+  </si>
+  <si>
     <t>Xinyi Glass Holdings</t>
   </si>
   <si>
+    <t>0883</t>
+  </si>
+  <si>
     <t>CNOOC</t>
   </si>
   <si>
+    <t>0939</t>
+  </si>
+  <si>
     <t>China Construction Bank</t>
   </si>
   <si>
+    <t>0941</t>
+  </si>
+  <si>
     <t>China Mobile</t>
   </si>
   <si>
+    <t>0960</t>
+  </si>
+  <si>
     <t>WH Group</t>
+  </si>
+  <si>
+    <t>0992</t>
   </si>
   <si>
     <t>Lenovo Group</t>
@@ -308,7 +383,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -318,25 +393,22 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -508,9 +580,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -590,7 +662,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -618,10 +690,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -877,9 +949,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1167,7 +1239,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1195,10 +1267,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1475,377 +1547,377 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="5">
+      <c r="A2" t="s" s="4">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="B2" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7"/>
+      <c r="C2" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="8">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7"/>
+      <c r="A3" t="s" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E4" s="7"/>
+      <c r="A4" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7"/>
+      <c r="A5" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="8">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="A6" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="8">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="A7" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E8" s="7"/>
+      <c r="A8" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7"/>
+      <c r="A9" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E10" s="7"/>
+      <c r="A10" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="8">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="A11" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="8">
+      <c r="A12" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s" s="7">
         <v>27</v>
       </c>
-      <c r="B12" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="C12" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="8">
-        <v>66</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E13" s="7"/>
+      <c r="A13" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="8">
-        <v>101</v>
-      </c>
-      <c r="B14" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7"/>
+      <c r="A14" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="8">
-        <v>388</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E15" s="7"/>
+      <c r="A15" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="8">
-        <v>688</v>
-      </c>
-      <c r="B16" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E16" s="7"/>
+      <c r="A16" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="8">
-        <v>700</v>
-      </c>
-      <c r="B17" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E17" s="7"/>
+      <c r="A17" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="8">
-        <v>762</v>
-      </c>
-      <c r="B18" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E18" s="7"/>
+      <c r="A18" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="8">
-        <v>823</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s" s="9">
-        <v>6</v>
+      <c r="A19" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E19" s="7"/>
     </row>
     <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="8">
-        <v>857</v>
-      </c>
-      <c r="B20" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s" s="9">
-        <v>6</v>
+      <c r="A20" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E20" s="7"/>
     </row>
     <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="8">
-        <v>868</v>
-      </c>
-      <c r="B21" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s" s="9">
-        <v>6</v>
+      <c r="A21" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E21" s="7"/>
     </row>
     <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="8">
-        <v>883</v>
-      </c>
-      <c r="B22" t="s" s="9">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s" s="9">
-        <v>6</v>
+      <c r="A22" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E22" s="7"/>
     </row>
     <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="8">
-        <v>939</v>
-      </c>
-      <c r="B23" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s" s="9">
-        <v>6</v>
+      <c r="A23" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E23" s="7"/>
     </row>
     <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="8">
-        <v>941</v>
-      </c>
-      <c r="B24" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="C24" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s" s="9">
-        <v>6</v>
+      <c r="A24" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s" s="7">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E24" s="7"/>
     </row>
     <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="8">
-        <v>960</v>
-      </c>
-      <c r="B25" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s" s="9">
-        <v>6</v>
+      <c r="A25" t="s" s="7">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E25" s="7"/>
     </row>
     <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="8">
-        <v>992</v>
-      </c>
-      <c r="B26" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s" s="9">
-        <v>6</v>
+      <c r="A26" t="s" s="7">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s" s="7">
+        <v>7</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -1853,361 +1925,361 @@
       <c r="A27" s="8">
         <v>1038</v>
       </c>
-      <c r="B27" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="B27" t="s" s="7">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" s="8">
         <v>1044</v>
       </c>
-      <c r="B28" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="B28" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" s="8">
         <v>1088</v>
       </c>
-      <c r="B29" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="C29" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E29" s="7"/>
+      <c r="B29" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" s="8">
         <v>1109</v>
       </c>
-      <c r="B30" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="C30" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="B30" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" s="8">
         <v>1113</v>
       </c>
-      <c r="B31" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="B31" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" s="8">
         <v>1177</v>
       </c>
-      <c r="B32" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E32" s="7"/>
+      <c r="B32" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" s="8">
         <v>1211</v>
       </c>
-      <c r="B33" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="C33" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E33" s="7"/>
+      <c r="B33" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" s="8">
         <v>1299</v>
       </c>
-      <c r="B34" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E34" s="7"/>
+      <c r="B34" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" s="8">
         <v>1378</v>
       </c>
-      <c r="B35" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="C35" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E35" s="7"/>
+      <c r="B35" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" s="8">
         <v>1398</v>
       </c>
-      <c r="B36" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E36" s="7"/>
+      <c r="B36" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" s="8">
         <v>1928</v>
       </c>
-      <c r="B37" t="s" s="9">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E37" s="7"/>
+      <c r="B37" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" ht="13.55" customHeight="1">
       <c r="A38" s="8">
         <v>1997</v>
       </c>
-      <c r="B38" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C38" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E38" s="7"/>
+      <c r="B38" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" ht="13.55" customHeight="1">
       <c r="A39" s="8">
         <v>2007</v>
       </c>
-      <c r="B39" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="C39" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="B39" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" ht="13.55" customHeight="1">
       <c r="A40" s="8">
         <v>2018</v>
       </c>
-      <c r="B40" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="C40" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D40" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="B40" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" ht="13.55" customHeight="1">
       <c r="A41" s="8">
         <v>2313</v>
       </c>
-      <c r="B41" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="C41" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D41" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E41" s="7"/>
+      <c r="B41" t="s" s="7">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" ht="13.55" customHeight="1">
       <c r="A42" s="8">
         <v>2318</v>
       </c>
-      <c r="B42" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="C42" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E42" s="7"/>
+      <c r="B42" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" ht="13.55" customHeight="1">
       <c r="A43" s="8">
         <v>2319</v>
       </c>
-      <c r="B43" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="C43" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E43" s="7"/>
+      <c r="B43" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" ht="13.55" customHeight="1">
       <c r="A44" s="8">
         <v>2382</v>
       </c>
-      <c r="B44" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="C44" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D44" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E44" s="7"/>
+      <c r="B44" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" ht="13.55" customHeight="1">
       <c r="A45" s="8">
         <v>2388</v>
       </c>
-      <c r="B45" t="s" s="9">
-        <v>49</v>
-      </c>
-      <c r="C45" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E45" s="7"/>
+      <c r="B45" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" ht="13.55" customHeight="1">
       <c r="A46" s="8">
         <v>2628</v>
       </c>
-      <c r="B46" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="B46" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" ht="13.55" customHeight="1">
       <c r="A47" s="8">
         <v>2688</v>
       </c>
-      <c r="B47" t="s" s="9">
-        <v>50</v>
-      </c>
-      <c r="C47" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D47" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E47" s="7"/>
+      <c r="B47" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="C47" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" ht="13.55" customHeight="1">
       <c r="A48" s="8">
         <v>3690</v>
       </c>
-      <c r="B48" t="s" s="9">
-        <v>51</v>
-      </c>
-      <c r="C48" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E48" s="7"/>
+      <c r="B48" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="C48" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" ht="13.55" customHeight="1">
       <c r="A49" s="8">
         <v>3888</v>
       </c>
-      <c r="B49" t="s" s="9">
-        <v>52</v>
-      </c>
-      <c r="C49" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E49" s="7"/>
+      <c r="B49" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="C49" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E49" s="6"/>
     </row>
     <row r="50" ht="13.55" customHeight="1">
       <c r="A50" s="8">
         <v>3988</v>
       </c>
-      <c r="B50" t="s" s="9">
-        <v>53</v>
-      </c>
-      <c r="C50" t="s" s="5">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="E50" s="7"/>
+      <c r="B50" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="E50" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>